<commit_message>
added category and read-xls api
</commit_message>
<xml_diff>
--- a/files/todo.xlsx
+++ b/files/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\xls_todo_enhancer\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A85255-1611-4104-9B68-90B01AE92CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D3C585-31AB-400D-86A6-63C3723133FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="20520" windowHeight="12850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6930" yWindow="1660" windowWidth="20520" windowHeight="12850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To-Do List" sheetId="1" r:id="rId1"/>
@@ -779,7 +779,7 @@
   <dimension ref="A1:Y1018"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -873,7 +873,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -901,7 +901,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -929,7 +929,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
         <v>17</v>
@@ -951,7 +951,7 @@
       </c>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>19</v>
@@ -971,7 +971,7 @@
       </c>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
@@ -995,7 +995,7 @@
       </c>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
         <v>22</v>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
         <v>23</v>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
         <v>24</v>
@@ -1056,7 +1056,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>25</v>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:25" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>26</v>
@@ -1099,7 +1099,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:25" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>27</v>
       </c>

</xml_diff>